<commit_message>
Mar23_ profile snapshot update
</commit_message>
<xml_diff>
--- a/Mar21_ProfileSnapshot.xlsx
+++ b/Mar21_ProfileSnapshot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhon Vincent Ramos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1689437-CAAF-4900-873C-2D443298DD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6199E40B-E4EA-483A-BEB0-38662F2CD038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t xml:space="preserve">Consultant Name: </t>
   </si>
@@ -113,10 +113,6 @@
 I contributed as one of the Backend Developer roles and it was my responsibility, specifically, to work on API calls and localization.</t>
   </si>
   <si>
-    <t xml:space="preserve">App Developer. 
-</t>
-  </si>
-  <si>
     <t>My team and I used Git for source control, code review, and pull requests.</t>
   </si>
   <si>
@@ -136,18 +132,12 @@
     <t>One year.</t>
   </si>
   <si>
-    <t>We used Swift in Xcode and JIRA.</t>
-  </si>
-  <si>
     <t>Senior App Developer.</t>
   </si>
   <si>
     <t>A year and a half.</t>
   </si>
   <si>
-    <t>Used Objective-C to transition into Swift code.</t>
-  </si>
-  <si>
     <t>Milawaukee, Wisconsin</t>
   </si>
   <si>
@@ -161,6 +151,21 @@
   </si>
   <si>
     <t>SourceTree for Git and Jenkins.</t>
+  </si>
+  <si>
+    <t>We were a team of four.
+Our group at the time was split like this: one Project Lead, one Frontend Developer, and two Backend Developers. The client, at the time, would consult with our Project Lead and our Lead would then relay the feedback to us.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used Objective-C to transition into Swift code. </t>
+  </si>
+  <si>
+    <t>We used Swift in Xcode and JIRA. SwiftyJSON.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">App Developer. 
+I contributed as a Backend Developer within my own project team. I worked with developing payment services and touch ID systems.
+</t>
   </si>
 </sst>
 </file>
@@ -320,25 +325,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -346,7 +351,10 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -363,7 +371,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -380,7 +388,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -397,7 +405,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -414,7 +422,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -431,7 +439,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -448,7 +456,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -465,7 +473,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -482,7 +490,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -499,7 +507,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -516,7 +524,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -545,9 +553,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -576,20 +581,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:K9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:K9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="0" tableBorderDxfId="12">
   <autoFilter ref="A3:K9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Project / Client / App name" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Location of Project (https://www.freemaptools.com/how-far-can-i-travel.htm  It shows you areas where you would live based on locations and costs)" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Commute Length Between Home and Project Address (also, Public Transit or Own Vehicle?) " dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2-3 Key Restaurants and/or Places You Enjoyed Around Projet Location (Museums, Shopping Malls, etc.)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Environment Type - The production environment and practices (Were they on Agile? Did they have TDD? How was documentation handled?)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Team Size and Break Down of Roles / Departments (And how did the consultant interact with the various teams? Project Manager, Product Owner, Quality Assurance/Testing Team, UI/UX teams, international teams)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Role Title and Major Responsibilities " dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="3rd Party Technologies Used (Interview Prep Matrix can help with this) " dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Leadership Style, if the profile states &quot;Lead&quot; or &quot;Senior&quot; on the Project (Use the &quot;Considerations&quot; doc to help with this)" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Duration of the Project" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Iteration of Technology Used (What versions of languages / libraries / technologies?)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Project / Client / App name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Location of Project (https://www.freemaptools.com/how-far-can-i-travel.htm  It shows you areas where you would live based on locations and costs)" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Commute Length Between Home and Project Address (also, Public Transit or Own Vehicle?) " dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2-3 Key Restaurants and/or Places You Enjoyed Around Projet Location (Museums, Shopping Malls, etc.)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Environment Type - The production environment and practices (Were they on Agile? Did they have TDD? How was documentation handled?)" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Team Size and Break Down of Roles / Departments (And how did the consultant interact with the various teams? Project Manager, Product Owner, Quality Assurance/Testing Team, UI/UX teams, international teams)" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Role Title and Major Responsibilities " dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="3rd Party Technologies Used (Interview Prep Matrix can help with this) " dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Leadership Style, if the profile states &quot;Lead&quot; or &quot;Senior&quot; on the Project (Use the &quot;Considerations&quot; doc to help with this)" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Duration of the Project" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Iteration of Technology Used (What versions of languages / libraries / technologies?)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -919,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
@@ -1029,69 +1034,71 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="G5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>

</xml_diff>